<commit_message>
Doladěn čas, vytvořena verze pro interní testování
</commit_message>
<xml_diff>
--- a/Jednotky.xlsx
+++ b/Jednotky.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uzivatel\00_AndroidProgramovani\MojeApky\Pickulacka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6794147-F8F0-4ECD-8495-3B1C94BEF432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20BF3C-67E9-4DC8-AFAB-1A1F10F42E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D372B61F-C7AE-45E3-8ED1-E4C495282854}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Fabie</t>
   </si>
@@ -62,51 +62,6 @@
     <t>Bžilion</t>
   </si>
   <si>
-    <r>
-      <t>dneska</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t> - takňák až to vyjde</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>pozdějc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t> - zhruba dneska</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>na pivko</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF202122"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t> - něco mezi třema a šesti hodinama</t>
-    </r>
-  </si>
-  <si>
     <t>Objem</t>
   </si>
   <si>
@@ -131,12 +86,6 @@
     <t>Ostatní</t>
   </si>
   <si>
-    <t>Jáchym</t>
-  </si>
-  <si>
-    <t>Jednotka bolesti</t>
-  </si>
-  <si>
     <t>Palec</t>
   </si>
   <si>
@@ -152,9 +101,6 @@
     <t>Fotbalové hřiště</t>
   </si>
   <si>
-    <t>Spotřeba Fabie</t>
-  </si>
-  <si>
     <t>Nádrž Fabie</t>
   </si>
   <si>
@@ -185,12 +131,6 @@
     <t>Plocha (zadává klient)</t>
   </si>
   <si>
-    <t>Více než 180, méně než 360</t>
-  </si>
-  <si>
-    <t>Zadat poslední tři příchody</t>
-  </si>
-  <si>
     <t>v litrech</t>
   </si>
   <si>
@@ -198,13 +138,22 @@
   </si>
   <si>
     <t>Čas (Otázka "Kolik máš času?")</t>
+  </si>
+  <si>
+    <t>pozdějc</t>
+  </si>
+  <si>
+    <t>Napivkon</t>
+  </si>
+  <si>
+    <t>dnesk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,13 +161,6 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF202122"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -251,7 +193,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -570,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B693EEA7-D62C-4E87-9B05-8C4CD1451321}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,36 +531,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f>2.54/100</f>
@@ -637,13 +579,13 @@
         <v>259213</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>7.29</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -664,21 +606,21 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>0.25</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <f>16.0036/100</f>
@@ -688,39 +630,36 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1">
         <f>24*60</f>
         <v>1440</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>3.4908999999999999</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1">
         <f>15.687*60</f>
         <v>941.21999999999991</v>
       </c>
-      <c r="I5" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -731,37 +670,31 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <f>123*B8</f>
         <v>12484.254000000001</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
+        <v>34</v>
+      </c>
+      <c r="F7" s="1">
+        <v>38.756</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>101.498</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F8" s="1">
         <v>2.34</v>
@@ -769,21 +702,21 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1201120.1000000001</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="F9" s="1">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>40075000</v>
@@ -791,7 +724,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B11">
         <f>B4*1000000</f>

</xml_diff>